<commit_message>
added category id column and manual ad data
</commit_message>
<xml_diff>
--- a/Research/Manual_Ad_Data-Compilation.xlsx
+++ b/Research/Manual_Ad_Data-Compilation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="218">
   <si>
     <t>Video Name</t>
   </si>
@@ -609,6 +609,75 @@
   </si>
   <si>
     <t>2085</t>
+  </si>
+  <si>
+    <t>Video Duration</t>
+  </si>
+  <si>
+    <t>Ad Duration</t>
+  </si>
+  <si>
+    <t>Ad Comment Total</t>
+  </si>
+  <si>
+    <t>3716111141</t>
+  </si>
+  <si>
+    <t>21124439</t>
+  </si>
+  <si>
+    <t>703302</t>
+  </si>
+  <si>
+    <t>1496937</t>
+  </si>
+  <si>
+    <t>2715572415</t>
+  </si>
+  <si>
+    <t>8908105</t>
+  </si>
+  <si>
+    <t>423800</t>
+  </si>
+  <si>
+    <t>298738</t>
+  </si>
+  <si>
+    <t>3188560433</t>
+  </si>
+  <si>
+    <t>11256966</t>
+  </si>
+  <si>
+    <t>709285</t>
+  </si>
+  <si>
+    <t>438613</t>
+  </si>
+  <si>
+    <t>3615413</t>
+  </si>
+  <si>
+    <t>114944</t>
+  </si>
+  <si>
+    <t>3442</t>
+  </si>
+  <si>
+    <t>13448</t>
+  </si>
+  <si>
+    <t>1889448</t>
+  </si>
+  <si>
+    <t>42000</t>
+  </si>
+  <si>
+    <t>7476</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=MOo9iJ8RYWM</t>
   </si>
 </sst>
 </file>
@@ -618,7 +687,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -641,6 +710,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -675,11 +751,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -696,9 +776,16 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1011,12 +1098,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:V64"/>
+  <dimension ref="A3:V72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="S22" sqref="S22"/>
+      <selection pane="bottomLeft" activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3363,6 +3450,378 @@
         <v>134</v>
       </c>
       <c r="V64" s="11"/>
+    </row>
+    <row r="67" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B67" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E67" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F67" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G67" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H67" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="I67" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="J67" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="K67" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L67" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="M67" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N67" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="O67" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="P67" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q67" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="R67" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="S67" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="T67" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="U67" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="68" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B68" s="14">
+        <v>43335.632783879228</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="F68" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="G68" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="H68" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="I68" s="12">
+        <v>227</v>
+      </c>
+      <c r="J68" s="12">
+        <v>79</v>
+      </c>
+      <c r="K68" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L68" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="M68" s="12">
+        <v>144407650</v>
+      </c>
+      <c r="N68" s="12">
+        <v>6</v>
+      </c>
+      <c r="O68" s="12">
+        <v>23</v>
+      </c>
+      <c r="P68" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q68" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="R68" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="S68" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="T68" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="U68" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B69" s="14">
+        <v>43335.632783879228</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E69" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F69" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="G69" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="H69" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="I69" s="12">
+        <v>301</v>
+      </c>
+      <c r="J69" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K69" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L69" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M69" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N69" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="O69" s="12">
+        <v>0</v>
+      </c>
+      <c r="P69" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q69" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="R69" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="S69" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="T69" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="U69" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B70" s="14">
+        <v>43335.632783879228</v>
+      </c>
+      <c r="C70" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="G70" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="H70" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="I70" s="12">
+        <v>270</v>
+      </c>
+      <c r="J70" s="12">
+        <v>60</v>
+      </c>
+      <c r="K70" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L70" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="M70" s="12">
+        <v>245050933</v>
+      </c>
+      <c r="N70" s="12">
+        <v>1500</v>
+      </c>
+      <c r="O70" s="12">
+        <v>1700</v>
+      </c>
+      <c r="P70" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q70" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="R70" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="S70" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="T70" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="U70" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B71" s="14">
+        <v>43335.632783879228</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E71" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="F71" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G71" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="H71" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="I71" s="12">
+        <v>832</v>
+      </c>
+      <c r="J71" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K71" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L71" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M71" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N71" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="O71" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P71" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q71" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="R71" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="S71" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="T71" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="U71" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="72" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B72" s="14">
+        <v>43335.632783879228</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E72" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="F72" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="G72" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="H72" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="I72" s="12">
+        <v>252</v>
+      </c>
+      <c r="J72" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K72" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="L72" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="M72" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N72" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="O72" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P72" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q72" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="R72" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="S72" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="T72" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="U72" s="12" t="s">
+        <v>134</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3407,8 +3866,13 @@
     <hyperlink ref="D62" r:id="rId39"/>
     <hyperlink ref="D63" r:id="rId40"/>
     <hyperlink ref="D64" r:id="rId41"/>
+    <hyperlink ref="D68" r:id="rId42"/>
+    <hyperlink ref="D69" r:id="rId43"/>
+    <hyperlink ref="D70" r:id="rId44"/>
+    <hyperlink ref="D71" r:id="rId45"/>
+    <hyperlink ref="D72" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId42"/>
+  <pageSetup orientation="portrait" r:id="rId47"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added data for the 25th of Aug
</commit_message>
<xml_diff>
--- a/Research/Manual_Ad_Data-Compilation.xlsx
+++ b/Research/Manual_Ad_Data-Compilation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="242">
   <si>
     <t>Video Name</t>
   </si>
@@ -678,6 +678,78 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=MOo9iJ8RYWM</t>
+  </si>
+  <si>
+    <t>3719765057</t>
+  </si>
+  <si>
+    <t>21147382</t>
+  </si>
+  <si>
+    <t>704104</t>
+  </si>
+  <si>
+    <t>1499285</t>
+  </si>
+  <si>
+    <t>2716588186</t>
+  </si>
+  <si>
+    <t>8913426</t>
+  </si>
+  <si>
+    <t>424036</t>
+  </si>
+  <si>
+    <t>298923</t>
+  </si>
+  <si>
+    <t>3191872297</t>
+  </si>
+  <si>
+    <t>11270333</t>
+  </si>
+  <si>
+    <t>710110</t>
+  </si>
+  <si>
+    <t>439260</t>
+  </si>
+  <si>
+    <t>3625551</t>
+  </si>
+  <si>
+    <t>115117</t>
+  </si>
+  <si>
+    <t>3447</t>
+  </si>
+  <si>
+    <t>13468</t>
+  </si>
+  <si>
+    <t>1892921</t>
+  </si>
+  <si>
+    <t>42043</t>
+  </si>
+  <si>
+    <t>2089</t>
+  </si>
+  <si>
+    <t>7478</t>
+  </si>
+  <si>
+    <t>Taco Bell</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Hulu Castle Rock</t>
+  </si>
+  <si>
+    <t>Undefined</t>
   </si>
 </sst>
 </file>
@@ -759,7 +831,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -776,6 +848,13 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1098,12 +1177,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:V72"/>
+  <dimension ref="A3:V80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C78" sqref="C78"/>
+      <selection pane="bottomLeft" activeCell="O79" sqref="O79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1121,7 +1200,7 @@
     <col min="12" max="12" width="57.36328125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.6328125" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.08984375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13" bestFit="1" customWidth="1"/>
@@ -3820,6 +3899,378 @@
         <v>83</v>
       </c>
       <c r="U72" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="75" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B75" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E75" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F75" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G75" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H75" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="I75" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="J75" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="K75" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="L75" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="M75" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="N75" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="O75" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="P75" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q75" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="R75" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="S75" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="T75" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="U75" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="76" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B76" s="19">
+        <v>43337.574999365512</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E76" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="F76" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="G76" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="H76" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="I76" s="17">
+        <v>227</v>
+      </c>
+      <c r="J76" s="17">
+        <v>15</v>
+      </c>
+      <c r="K76" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="L76" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="M76" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N76" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O76" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P76" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q76" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="R76" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="S76" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="T76" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="U76" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B77" s="19">
+        <v>43337.574999365512</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E77" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="F77" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="G77" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="H77" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="I77" s="17">
+        <v>301</v>
+      </c>
+      <c r="J77" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K77" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L77" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M77" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N77" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O77" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P77" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q77" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="R77" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="S77" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="T77" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="U77" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B78" s="19">
+        <v>43337.574999365512</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D78" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E78" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="F78" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="G78" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="H78" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="I78" s="17">
+        <v>270</v>
+      </c>
+      <c r="J78" s="17">
+        <v>15</v>
+      </c>
+      <c r="K78" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="L78" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M78" s="17">
+        <v>535975</v>
+      </c>
+      <c r="N78" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O78" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P78" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q78" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="R78" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="S78" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="T78" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="U78" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="79" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B79" s="19">
+        <v>43337.574999365512</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E79" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="F79" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="G79" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="H79" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="I79" s="17">
+        <v>832</v>
+      </c>
+      <c r="J79" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K79" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="L79" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M79" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N79" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O79" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P79" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q79" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="R79" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="S79" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="T79" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="U79" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="80" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B80" s="19">
+        <v>43337.574999365512</v>
+      </c>
+      <c r="C80" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D80" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E80" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="F80" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="G80" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="H80" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="I80" s="17">
+        <v>252</v>
+      </c>
+      <c r="J80" s="17">
+        <v>15</v>
+      </c>
+      <c r="K80" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="L80" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="M80" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N80" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O80" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P80" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q80" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="R80" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="S80" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="T80" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="U80" s="17" t="s">
         <v>134</v>
       </c>
     </row>
@@ -3871,8 +4322,13 @@
     <hyperlink ref="D70" r:id="rId44"/>
     <hyperlink ref="D71" r:id="rId45"/>
     <hyperlink ref="D72" r:id="rId46"/>
+    <hyperlink ref="D76" r:id="rId47"/>
+    <hyperlink ref="D77" r:id="rId48"/>
+    <hyperlink ref="D78" r:id="rId49"/>
+    <hyperlink ref="D79" r:id="rId50"/>
+    <hyperlink ref="D80" r:id="rId51"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId47"/>
+  <pageSetup orientation="portrait" r:id="rId52"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added data for Aug 26th
</commit_message>
<xml_diff>
--- a/Research/Manual_Ad_Data-Compilation.xlsx
+++ b/Research/Manual_Ad_Data-Compilation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="263">
   <si>
     <t>Video Name</t>
   </si>
@@ -750,6 +750,69 @@
   </si>
   <si>
     <t>Undefined</t>
+  </si>
+  <si>
+    <t>3721733813</t>
+  </si>
+  <si>
+    <t>21160383</t>
+  </si>
+  <si>
+    <t>704537</t>
+  </si>
+  <si>
+    <t>1500376</t>
+  </si>
+  <si>
+    <t>2717129411</t>
+  </si>
+  <si>
+    <t>8916272</t>
+  </si>
+  <si>
+    <t>424189</t>
+  </si>
+  <si>
+    <t>299078</t>
+  </si>
+  <si>
+    <t>3193818485</t>
+  </si>
+  <si>
+    <t>11278842</t>
+  </si>
+  <si>
+    <t>710647</t>
+  </si>
+  <si>
+    <t>439567</t>
+  </si>
+  <si>
+    <t>3630197</t>
+  </si>
+  <si>
+    <t>115204</t>
+  </si>
+  <si>
+    <t>13469</t>
+  </si>
+  <si>
+    <t>1894654</t>
+  </si>
+  <si>
+    <t>42062</t>
+  </si>
+  <si>
+    <t>7479</t>
+  </si>
+  <si>
+    <t>Hulu</t>
+  </si>
+  <si>
+    <t>PPG Paints</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=</t>
   </si>
 </sst>
 </file>
@@ -1177,12 +1240,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:V80"/>
+  <dimension ref="A3:V88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="O79" sqref="O79"/>
+      <selection pane="bottomLeft" activeCell="P61" sqref="P61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3333,6 +3396,27 @@
       <c r="I60" s="9">
         <v>227</v>
       </c>
+      <c r="J60">
+        <v>15</v>
+      </c>
+      <c r="K60" t="s">
+        <v>261</v>
+      </c>
+      <c r="L60" t="s">
+        <v>262</v>
+      </c>
+      <c r="M60" s="4">
+        <v>21767861</v>
+      </c>
+      <c r="N60" s="4">
+        <v>32</v>
+      </c>
+      <c r="O60" s="4">
+        <v>18</v>
+      </c>
+      <c r="P60" s="4">
+        <v>4</v>
+      </c>
       <c r="Q60" s="9" t="s">
         <v>45</v>
       </c>
@@ -3378,6 +3462,27 @@
       <c r="I61" s="9">
         <v>301</v>
       </c>
+      <c r="J61" t="s">
+        <v>15</v>
+      </c>
+      <c r="K61" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L61" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M61" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N61" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O61" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P61" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="Q61" s="9" t="s">
         <v>53</v>
       </c>
@@ -3423,6 +3528,27 @@
       <c r="I62" s="9">
         <v>270</v>
       </c>
+      <c r="J62" t="s">
+        <v>15</v>
+      </c>
+      <c r="K62" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L62" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M62" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N62" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O62" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P62" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="Q62" s="9" t="s">
         <v>61</v>
       </c>
@@ -3468,6 +3594,27 @@
       <c r="I63" s="9">
         <v>832</v>
       </c>
+      <c r="J63" t="s">
+        <v>15</v>
+      </c>
+      <c r="K63" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L63" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M63" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N63" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O63" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P63" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="Q63" s="9" t="s">
         <v>69</v>
       </c>
@@ -3513,6 +3660,27 @@
       <c r="I64" s="9">
         <v>252</v>
       </c>
+      <c r="J64">
+        <v>15</v>
+      </c>
+      <c r="K64" t="s">
+        <v>260</v>
+      </c>
+      <c r="L64" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M64" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N64" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O64" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P64" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="Q64" s="9" t="s">
         <v>77</v>
       </c>
@@ -4271,6 +4439,378 @@
         <v>83</v>
       </c>
       <c r="U80" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="83" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B83" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D83" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E83" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F83" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G83" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H83" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="I83" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="J83" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="K83" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="L83" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="M83" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="N83" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="O83" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="P83" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q83" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="R83" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="S83" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="T83" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="U83" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="84" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B84" s="19">
+        <v>43338.628139433073</v>
+      </c>
+      <c r="C84" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D84" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E84" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="F84" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="G84" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="H84" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="I84" s="17">
+        <v>227</v>
+      </c>
+      <c r="J84" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K84" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L84" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M84" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N84" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O84" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P84" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q84" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="R84" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="S84" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="T84" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="U84" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="85" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B85" s="19">
+        <v>43338.628139433073</v>
+      </c>
+      <c r="C85" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D85" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E85" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="F85" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="G85" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="H85" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="I85" s="17">
+        <v>301</v>
+      </c>
+      <c r="J85" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K85" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L85" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M85" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N85" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O85" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P85" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q85" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="R85" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="S85" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="T85" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="U85" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="86" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B86" s="19">
+        <v>43338.628139433073</v>
+      </c>
+      <c r="C86" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D86" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E86" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="F86" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="G86" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="H86" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="I86" s="17">
+        <v>270</v>
+      </c>
+      <c r="J86" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K86" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L86" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M86" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N86" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O86" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P86" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q86" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="R86" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="S86" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="T86" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="U86" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="87" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B87" s="19">
+        <v>43338.628139433073</v>
+      </c>
+      <c r="C87" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D87" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E87" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="F87" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="G87" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="H87" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="I87" s="17">
+        <v>832</v>
+      </c>
+      <c r="J87" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K87" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L87" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M87" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N87" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O87" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P87" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q87" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="R87" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="S87" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="T87" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="U87" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="88" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B88" s="19">
+        <v>43338.628139433073</v>
+      </c>
+      <c r="C88" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D88" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E88" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="F88" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="G88" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="H88" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="I88" s="17">
+        <v>252</v>
+      </c>
+      <c r="J88" s="17">
+        <v>15</v>
+      </c>
+      <c r="K88" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="L88" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M88" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N88" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O88" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P88" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q88" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="R88" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="S88" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="T88" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="U88" s="17" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4327,8 +4867,13 @@
     <hyperlink ref="D78" r:id="rId49"/>
     <hyperlink ref="D79" r:id="rId50"/>
     <hyperlink ref="D80" r:id="rId51"/>
+    <hyperlink ref="D84" r:id="rId52"/>
+    <hyperlink ref="D85" r:id="rId53"/>
+    <hyperlink ref="D86" r:id="rId54"/>
+    <hyperlink ref="D87" r:id="rId55"/>
+    <hyperlink ref="D88" r:id="rId56"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId52"/>
+  <pageSetup orientation="portrait" r:id="rId57"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added data for 27th and 28th of August
</commit_message>
<xml_diff>
--- a/Research/Manual_Ad_Data-Compilation.xlsx
+++ b/Research/Manual_Ad_Data-Compilation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="301">
   <si>
     <t>Video Name</t>
   </si>
@@ -813,6 +813,120 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=</t>
+  </si>
+  <si>
+    <t>McDonald's</t>
+  </si>
+  <si>
+    <t>3724136968</t>
+  </si>
+  <si>
+    <t>21175356</t>
+  </si>
+  <si>
+    <t>705060</t>
+  </si>
+  <si>
+    <t>1501616</t>
+  </si>
+  <si>
+    <t>2717762439</t>
+  </si>
+  <si>
+    <t>8919656</t>
+  </si>
+  <si>
+    <t>424326</t>
+  </si>
+  <si>
+    <t>299240</t>
+  </si>
+  <si>
+    <t>3196114271</t>
+  </si>
+  <si>
+    <t>11288637</t>
+  </si>
+  <si>
+    <t>711245</t>
+  </si>
+  <si>
+    <t>439862</t>
+  </si>
+  <si>
+    <t>3637821</t>
+  </si>
+  <si>
+    <t>115330</t>
+  </si>
+  <si>
+    <t>3448</t>
+  </si>
+  <si>
+    <t>13472</t>
+  </si>
+  <si>
+    <t>1897020</t>
+  </si>
+  <si>
+    <t>42084</t>
+  </si>
+  <si>
+    <t>2090</t>
+  </si>
+  <si>
+    <t>3725029276</t>
+  </si>
+  <si>
+    <t>21181573</t>
+  </si>
+  <si>
+    <t>705226</t>
+  </si>
+  <si>
+    <t>1502109</t>
+  </si>
+  <si>
+    <t>2718200219</t>
+  </si>
+  <si>
+    <t>8922109</t>
+  </si>
+  <si>
+    <t>424430</t>
+  </si>
+  <si>
+    <t>299306</t>
+  </si>
+  <si>
+    <t>3196753727</t>
+  </si>
+  <si>
+    <t>11291756</t>
+  </si>
+  <si>
+    <t>711463</t>
+  </si>
+  <si>
+    <t>439969</t>
+  </si>
+  <si>
+    <t>3641003</t>
+  </si>
+  <si>
+    <t>115369</t>
+  </si>
+  <si>
+    <t>13474</t>
+  </si>
+  <si>
+    <t>1897686</t>
+  </si>
+  <si>
+    <t>42093</t>
+  </si>
+  <si>
+    <t>2091</t>
   </si>
 </sst>
 </file>
@@ -1240,12 +1354,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:V88"/>
+  <dimension ref="A3:AB104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="P61" sqref="P61"/>
+      <selection pane="bottomLeft" activeCell="I99" sqref="I99:AB104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3128,6 +3242,27 @@
       <c r="I53" s="9">
         <v>227</v>
       </c>
+      <c r="J53">
+        <v>30</v>
+      </c>
+      <c r="K53" t="s">
+        <v>263</v>
+      </c>
+      <c r="L53" t="s">
+        <v>15</v>
+      </c>
+      <c r="M53" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N53" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O53" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P53" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="Q53" s="9" t="s">
         <v>45</v>
       </c>
@@ -3173,6 +3308,27 @@
       <c r="I54" s="9">
         <v>301</v>
       </c>
+      <c r="J54" t="s">
+        <v>15</v>
+      </c>
+      <c r="K54" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L54" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M54" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N54" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O54" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P54" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="Q54" s="9" t="s">
         <v>53</v>
       </c>
@@ -3218,6 +3374,27 @@
       <c r="I55" s="9">
         <v>270</v>
       </c>
+      <c r="J55">
+        <v>60</v>
+      </c>
+      <c r="K55" t="s">
+        <v>26</v>
+      </c>
+      <c r="L55" t="s">
+        <v>217</v>
+      </c>
+      <c r="M55" s="4">
+        <v>246542786</v>
+      </c>
+      <c r="N55" s="4">
+        <v>1500</v>
+      </c>
+      <c r="O55" s="4">
+        <v>1700</v>
+      </c>
+      <c r="P55" t="s">
+        <v>15</v>
+      </c>
       <c r="Q55" s="9" t="s">
         <v>61</v>
       </c>
@@ -3263,6 +3440,27 @@
       <c r="I56" s="9">
         <v>832</v>
       </c>
+      <c r="J56" t="s">
+        <v>15</v>
+      </c>
+      <c r="K56" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L56" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M56" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N56" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O56" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P56" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="Q56" s="9" t="s">
         <v>69</v>
       </c>
@@ -3308,6 +3506,27 @@
       <c r="I57" s="9">
         <v>252</v>
       </c>
+      <c r="J57">
+        <v>15</v>
+      </c>
+      <c r="K57" t="s">
+        <v>260</v>
+      </c>
+      <c r="L57" t="s">
+        <v>15</v>
+      </c>
+      <c r="M57" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N57" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O57" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P57" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="Q57" s="9" t="s">
         <v>77</v>
       </c>
@@ -4811,6 +5030,750 @@
         <v>83</v>
       </c>
       <c r="U88" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="91" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B91" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C91" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D91" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E91" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F91" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G91" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H91" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="I91" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="J91" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="K91" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="L91" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="M91" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="N91" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="O91" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="P91" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q91" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="R91" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="S91" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="T91" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="U91" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="92" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B92" s="19">
+        <v>43339.981719309813</v>
+      </c>
+      <c r="C92" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D92" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E92" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="F92" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="G92" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="H92" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="I92" s="17">
+        <v>227</v>
+      </c>
+      <c r="J92" s="17">
+        <v>60</v>
+      </c>
+      <c r="K92" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="L92" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="M92" s="17">
+        <v>247385363</v>
+      </c>
+      <c r="N92" s="17">
+        <v>1500</v>
+      </c>
+      <c r="O92" s="17">
+        <v>1700</v>
+      </c>
+      <c r="P92" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q92" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="R92" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="S92" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="T92" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="U92" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="93" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B93" s="19">
+        <v>43339.981719309813</v>
+      </c>
+      <c r="C93" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D93" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E93" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="F93" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="G93" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="H93" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="I93" s="17">
+        <v>301</v>
+      </c>
+      <c r="J93" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K93" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L93" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M93" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N93" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O93" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P93" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q93" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="R93" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="S93" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="T93" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="U93" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="94" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B94" s="19">
+        <v>43339.981719309813</v>
+      </c>
+      <c r="C94" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D94" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E94" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="F94" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="G94" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="H94" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="I94" s="17">
+        <v>270</v>
+      </c>
+      <c r="J94" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K94" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L94" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M94" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N94" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O94" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P94" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q94" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="R94" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="S94" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="T94" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="U94" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="95" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B95" s="19">
+        <v>43339.981719309813</v>
+      </c>
+      <c r="C95" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D95" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E95" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="F95" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="G95" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="H95" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="I95" s="17">
+        <v>832</v>
+      </c>
+      <c r="J95" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K95" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L95" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M95" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N95" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O95" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P95" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q95" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="R95" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="S95" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="T95" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="U95" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="96" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B96" s="19">
+        <v>43339.981719309813</v>
+      </c>
+      <c r="C96" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D96" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E96" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="F96" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="G96" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="H96" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="I96" s="17">
+        <v>252</v>
+      </c>
+      <c r="J96" s="17">
+        <v>15</v>
+      </c>
+      <c r="K96" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="L96" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M96" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N96" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O96" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P96" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q96" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="R96" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="S96" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="T96" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="U96" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="99" spans="9:28" x14ac:dyDescent="0.35">
+      <c r="I99" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J99" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K99" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="L99" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="M99" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="N99" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="O99" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="P99" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q99" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="R99" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="S99" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="T99" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="U99" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="V99" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="W99" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="X99" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y99" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z99" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA99" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB99" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="100" spans="9:28" x14ac:dyDescent="0.35">
+      <c r="I100" s="19">
+        <v>43340.504598848493</v>
+      </c>
+      <c r="J100" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K100" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="L100" s="17" t="s">
+        <v>283</v>
+      </c>
+      <c r="M100" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="N100" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="O100" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="P100" s="17">
+        <v>227</v>
+      </c>
+      <c r="Q100" s="17">
+        <v>0</v>
+      </c>
+      <c r="R100" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="S100" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="T100" s="17">
+        <v>0</v>
+      </c>
+      <c r="U100" s="17">
+        <v>0</v>
+      </c>
+      <c r="V100" s="17">
+        <v>0</v>
+      </c>
+      <c r="W100" s="17">
+        <v>0</v>
+      </c>
+      <c r="X100" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y100" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z100" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA100" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB100" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="101" spans="9:28" x14ac:dyDescent="0.35">
+      <c r="I101" s="19">
+        <v>43340.504598848493</v>
+      </c>
+      <c r="J101" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K101" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="L101" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="M101" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="N101" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="O101" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="P101" s="17">
+        <v>301</v>
+      </c>
+      <c r="Q101" s="17">
+        <v>0</v>
+      </c>
+      <c r="R101" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="S101" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="T101" s="17">
+        <v>0</v>
+      </c>
+      <c r="U101" s="17">
+        <v>0</v>
+      </c>
+      <c r="V101" s="17">
+        <v>0</v>
+      </c>
+      <c r="W101" s="17">
+        <v>0</v>
+      </c>
+      <c r="X101" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y101" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z101" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA101" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB101" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="102" spans="9:28" x14ac:dyDescent="0.35">
+      <c r="I102" s="19">
+        <v>43340.504598848493</v>
+      </c>
+      <c r="J102" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="K102" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="L102" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="M102" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="N102" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="O102" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="P102" s="17">
+        <v>270</v>
+      </c>
+      <c r="Q102" s="17">
+        <v>0</v>
+      </c>
+      <c r="R102" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="S102" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="T102" s="17">
+        <v>0</v>
+      </c>
+      <c r="U102" s="17">
+        <v>0</v>
+      </c>
+      <c r="V102" s="17">
+        <v>0</v>
+      </c>
+      <c r="W102" s="17">
+        <v>0</v>
+      </c>
+      <c r="X102" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y102" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z102" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA102" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB102" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="103" spans="9:28" x14ac:dyDescent="0.35">
+      <c r="I103" s="19">
+        <v>43340.504598848493</v>
+      </c>
+      <c r="J103" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="K103" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="L103" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="M103" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="N103" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="O103" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="P103" s="17">
+        <v>832</v>
+      </c>
+      <c r="Q103" s="17">
+        <v>0</v>
+      </c>
+      <c r="R103" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="S103" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="T103" s="17">
+        <v>0</v>
+      </c>
+      <c r="U103" s="17">
+        <v>0</v>
+      </c>
+      <c r="V103" s="17">
+        <v>0</v>
+      </c>
+      <c r="W103" s="17">
+        <v>0</v>
+      </c>
+      <c r="X103" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y103" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z103" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA103" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB103" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="104" spans="9:28" x14ac:dyDescent="0.35">
+      <c r="I104" s="19">
+        <v>43340.504598848493</v>
+      </c>
+      <c r="J104" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="K104" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="L104" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="M104" s="17" t="s">
+        <v>299</v>
+      </c>
+      <c r="N104" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="O104" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="P104" s="17">
+        <v>252</v>
+      </c>
+      <c r="Q104" s="17">
+        <v>0</v>
+      </c>
+      <c r="R104" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="S104" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="T104" s="17">
+        <v>0</v>
+      </c>
+      <c r="U104" s="17">
+        <v>0</v>
+      </c>
+      <c r="V104" s="17">
+        <v>0</v>
+      </c>
+      <c r="W104" s="17">
+        <v>0</v>
+      </c>
+      <c r="X104" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y104" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z104" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA104" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB104" s="17" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4872,8 +5835,19 @@
     <hyperlink ref="D86" r:id="rId54"/>
     <hyperlink ref="D87" r:id="rId55"/>
     <hyperlink ref="D88" r:id="rId56"/>
+    <hyperlink ref="D92" r:id="rId57"/>
+    <hyperlink ref="D93" r:id="rId58"/>
+    <hyperlink ref="D94" r:id="rId59"/>
+    <hyperlink ref="D95" r:id="rId60"/>
+    <hyperlink ref="D96" r:id="rId61"/>
+    <hyperlink ref="L92" r:id="rId62"/>
+    <hyperlink ref="K100" r:id="rId63"/>
+    <hyperlink ref="K101" r:id="rId64"/>
+    <hyperlink ref="K102" r:id="rId65"/>
+    <hyperlink ref="K103" r:id="rId66"/>
+    <hyperlink ref="K104" r:id="rId67"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId57"/>
+  <pageSetup orientation="portrait" r:id="rId68"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Data for early september
</commit_message>
<xml_diff>
--- a/Research/Manual_Ad_Data-Compilation.xlsx
+++ b/Research/Manual_Ad_Data-Compilation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="368">
   <si>
     <t>Video Name</t>
   </si>
@@ -993,6 +993,141 @@
   </si>
   <si>
     <t>Adidas</t>
+  </si>
+  <si>
+    <t>3734610957</t>
+  </si>
+  <si>
+    <t>21250323</t>
+  </si>
+  <si>
+    <t>707288</t>
+  </si>
+  <si>
+    <t>1507691</t>
+  </si>
+  <si>
+    <t>2725144101</t>
+  </si>
+  <si>
+    <t>8954051</t>
+  </si>
+  <si>
+    <t>425734</t>
+  </si>
+  <si>
+    <t>300368</t>
+  </si>
+  <si>
+    <t>3207058884</t>
+  </si>
+  <si>
+    <t>11336514</t>
+  </si>
+  <si>
+    <t>714103</t>
+  </si>
+  <si>
+    <t>441587</t>
+  </si>
+  <si>
+    <t>3688573</t>
+  </si>
+  <si>
+    <t>116067</t>
+  </si>
+  <si>
+    <t>3460</t>
+  </si>
+  <si>
+    <t>13585</t>
+  </si>
+  <si>
+    <t>1904887</t>
+  </si>
+  <si>
+    <t>42171</t>
+  </si>
+  <si>
+    <t>7484</t>
+  </si>
+  <si>
+    <t>toofaced</t>
+  </si>
+  <si>
+    <t>Billie Eilish</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=6KXAzmFAEKg&amp;index=2&amp;list=PL9tY0BWXOZFvyS_TIUi_YzYi9-n2u5r-t</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=DcrqBv1ty3w</t>
+  </si>
+  <si>
+    <t>3737422564</t>
+  </si>
+  <si>
+    <t>21267993</t>
+  </si>
+  <si>
+    <t>707835</t>
+  </si>
+  <si>
+    <t>1509377</t>
+  </si>
+  <si>
+    <t>2726653257</t>
+  </si>
+  <si>
+    <t>8960825</t>
+  </si>
+  <si>
+    <t>426010</t>
+  </si>
+  <si>
+    <t>300594</t>
+  </si>
+  <si>
+    <t>3209574958</t>
+  </si>
+  <si>
+    <t>11347006</t>
+  </si>
+  <si>
+    <t>714744</t>
+  </si>
+  <si>
+    <t>442062</t>
+  </si>
+  <si>
+    <t>3703036</t>
+  </si>
+  <si>
+    <t>116267</t>
+  </si>
+  <si>
+    <t>3462</t>
+  </si>
+  <si>
+    <t>13597</t>
+  </si>
+  <si>
+    <t>1906732</t>
+  </si>
+  <si>
+    <t>42190</t>
+  </si>
+  <si>
+    <t>2092</t>
+  </si>
+  <si>
+    <t>7485</t>
+  </si>
+  <si>
+    <t>Takis</t>
+  </si>
+  <si>
+    <t>Nissan</t>
   </si>
 </sst>
 </file>
@@ -1421,12 +1556,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AB112"/>
+  <dimension ref="A3:AB128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="P108" sqref="P108:P112"/>
+      <selection pane="bottomLeft" activeCell="O134" sqref="O134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3036,6 +3171,27 @@
       <c r="I45" s="9">
         <v>227</v>
       </c>
+      <c r="J45">
+        <v>80</v>
+      </c>
+      <c r="K45" t="s">
+        <v>112</v>
+      </c>
+      <c r="L45" t="s">
+        <v>113</v>
+      </c>
+      <c r="M45" s="4">
+        <v>149643705</v>
+      </c>
+      <c r="N45" s="4">
+        <v>6</v>
+      </c>
+      <c r="O45" s="4">
+        <v>26</v>
+      </c>
+      <c r="P45" t="s">
+        <v>15</v>
+      </c>
       <c r="Q45" s="9" t="s">
         <v>45</v>
       </c>
@@ -3081,6 +3237,27 @@
       <c r="I46" s="9">
         <v>301</v>
       </c>
+      <c r="J46">
+        <v>15</v>
+      </c>
+      <c r="K46" t="s">
+        <v>342</v>
+      </c>
+      <c r="L46" t="s">
+        <v>345</v>
+      </c>
+      <c r="M46" s="4">
+        <v>3772573</v>
+      </c>
+      <c r="N46" s="4">
+        <v>0</v>
+      </c>
+      <c r="O46" s="4">
+        <v>0</v>
+      </c>
+      <c r="P46" s="4">
+        <v>0</v>
+      </c>
       <c r="Q46" s="9" t="s">
         <v>53</v>
       </c>
@@ -3126,6 +3303,27 @@
       <c r="I47" s="9">
         <v>270</v>
       </c>
+      <c r="J47">
+        <v>13</v>
+      </c>
+      <c r="K47" t="s">
+        <v>343</v>
+      </c>
+      <c r="L47" t="s">
+        <v>344</v>
+      </c>
+      <c r="M47" s="4">
+        <v>1015023</v>
+      </c>
+      <c r="N47" s="4">
+        <v>100000</v>
+      </c>
+      <c r="O47" s="4">
+        <v>483</v>
+      </c>
+      <c r="P47" s="4">
+        <v>4281</v>
+      </c>
       <c r="Q47" s="9" t="s">
         <v>61</v>
       </c>
@@ -3171,6 +3369,27 @@
       <c r="I48" s="9">
         <v>832</v>
       </c>
+      <c r="J48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K48" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L48" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M48" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N48" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O48" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P48" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="Q48" s="9" t="s">
         <v>69</v>
       </c>
@@ -3215,6 +3434,27 @@
       </c>
       <c r="I49" s="9">
         <v>252</v>
+      </c>
+      <c r="J49" t="s">
+        <v>15</v>
+      </c>
+      <c r="K49" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L49" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M49" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N49" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O49" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P49" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="Q49" s="9" t="s">
         <v>77</v>
@@ -6255,6 +6495,750 @@
         <v>83</v>
       </c>
       <c r="U112" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="115" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B115" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C115" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D115" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E115" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F115" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G115" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H115" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="I115" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="J115" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="K115" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="L115" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="M115" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="N115" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="O115" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="P115" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q115" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="R115" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="S115" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="T115" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="U115" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="116" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B116" s="19">
+        <v>43345.65389642318</v>
+      </c>
+      <c r="C116" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D116" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E116" s="17" t="s">
+        <v>323</v>
+      </c>
+      <c r="F116" s="17" t="s">
+        <v>324</v>
+      </c>
+      <c r="G116" s="17" t="s">
+        <v>325</v>
+      </c>
+      <c r="H116" s="17" t="s">
+        <v>326</v>
+      </c>
+      <c r="I116" s="17">
+        <v>227</v>
+      </c>
+      <c r="J116" s="17">
+        <v>60</v>
+      </c>
+      <c r="K116" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="L116" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="M116" s="17">
+        <v>247388342</v>
+      </c>
+      <c r="N116" s="17">
+        <v>1500</v>
+      </c>
+      <c r="O116" s="17">
+        <v>1700</v>
+      </c>
+      <c r="P116" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q116" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="R116" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="S116" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="T116" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="U116" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="117" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B117" s="19">
+        <v>43345.65389642318</v>
+      </c>
+      <c r="C117" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D117" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E117" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="F117" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="G117" s="17" t="s">
+        <v>329</v>
+      </c>
+      <c r="H117" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="I117" s="17">
+        <v>301</v>
+      </c>
+      <c r="J117" s="17">
+        <v>0</v>
+      </c>
+      <c r="K117" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L117" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M117" s="17">
+        <v>0</v>
+      </c>
+      <c r="N117" s="17">
+        <v>0</v>
+      </c>
+      <c r="O117" s="17">
+        <v>0</v>
+      </c>
+      <c r="P117" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q117" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="R117" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="S117" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="T117" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="U117" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="118" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B118" s="19">
+        <v>43345.65389642318</v>
+      </c>
+      <c r="C118" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D118" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E118" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="F118" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="G118" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="H118" s="17" t="s">
+        <v>334</v>
+      </c>
+      <c r="I118" s="17">
+        <v>270</v>
+      </c>
+      <c r="J118" s="17">
+        <v>0</v>
+      </c>
+      <c r="K118" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L118" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M118" s="17">
+        <v>0</v>
+      </c>
+      <c r="N118" s="17">
+        <v>0</v>
+      </c>
+      <c r="O118" s="17">
+        <v>0</v>
+      </c>
+      <c r="P118" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q118" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="R118" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="S118" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="T118" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="U118" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="119" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B119" s="19">
+        <v>43345.65389642318</v>
+      </c>
+      <c r="C119" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D119" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E119" s="17" t="s">
+        <v>335</v>
+      </c>
+      <c r="F119" s="17" t="s">
+        <v>336</v>
+      </c>
+      <c r="G119" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="H119" s="17" t="s">
+        <v>338</v>
+      </c>
+      <c r="I119" s="17">
+        <v>832</v>
+      </c>
+      <c r="J119" s="17">
+        <v>0</v>
+      </c>
+      <c r="K119" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L119" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M119" s="17">
+        <v>0</v>
+      </c>
+      <c r="N119" s="17">
+        <v>0</v>
+      </c>
+      <c r="O119" s="17">
+        <v>0</v>
+      </c>
+      <c r="P119" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q119" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="R119" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="S119" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="T119" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="U119" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="120" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B120" s="19">
+        <v>43345.65389642318</v>
+      </c>
+      <c r="C120" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D120" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E120" s="17" t="s">
+        <v>339</v>
+      </c>
+      <c r="F120" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="G120" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="H120" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="I120" s="17">
+        <v>252</v>
+      </c>
+      <c r="J120" s="17">
+        <v>0</v>
+      </c>
+      <c r="K120" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L120" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M120" s="17">
+        <v>0</v>
+      </c>
+      <c r="N120" s="17">
+        <v>0</v>
+      </c>
+      <c r="O120" s="17">
+        <v>0</v>
+      </c>
+      <c r="P120" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q120" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="R120" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="S120" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="T120" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="U120" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="123" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B123" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C123" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D123" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E123" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="F123" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G123" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="H123" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="I123" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="J123" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="K123" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="L123" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="M123" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="N123" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="O123" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="P123" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q123" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="R123" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="S123" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="T123" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="U123" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="124" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B124" s="19">
+        <v>43346.998384863648</v>
+      </c>
+      <c r="C124" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D124" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E124" s="17" t="s">
+        <v>346</v>
+      </c>
+      <c r="F124" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="G124" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="H124" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="I124" s="17">
+        <v>227</v>
+      </c>
+      <c r="J124" s="17">
+        <v>60</v>
+      </c>
+      <c r="K124" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="L124" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="M124" s="17">
+        <v>253678786</v>
+      </c>
+      <c r="N124" s="17">
+        <v>1600</v>
+      </c>
+      <c r="O124" s="17">
+        <v>1800</v>
+      </c>
+      <c r="P124" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q124" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="R124" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="S124" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="T124" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="U124" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="125" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B125" s="19">
+        <v>43346.998384863648</v>
+      </c>
+      <c r="C125" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D125" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E125" s="17" t="s">
+        <v>350</v>
+      </c>
+      <c r="F125" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="G125" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="H125" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="I125" s="17">
+        <v>301</v>
+      </c>
+      <c r="J125" s="17">
+        <v>15</v>
+      </c>
+      <c r="K125" s="17" t="s">
+        <v>366</v>
+      </c>
+      <c r="L125" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M125" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N125" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O125" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P125" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q125" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="R125" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="S125" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="T125" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="U125" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="126" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B126" s="19">
+        <v>43346.998384863648</v>
+      </c>
+      <c r="C126" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D126" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E126" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="F126" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="G126" s="17" t="s">
+        <v>356</v>
+      </c>
+      <c r="H126" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="I126" s="17">
+        <v>270</v>
+      </c>
+      <c r="J126" s="17">
+        <v>15</v>
+      </c>
+      <c r="K126" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="L126" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M126" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N126" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O126" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P126" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q126" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="R126" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="S126" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="T126" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="U126" s="17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="127" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B127" s="19">
+        <v>43346.998384863648</v>
+      </c>
+      <c r="C127" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D127" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E127" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="F127" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="G127" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="H127" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="I127" s="17">
+        <v>832</v>
+      </c>
+      <c r="J127" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K127" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L127" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M127" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N127" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O127" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P127" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q127" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="R127" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="S127" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="T127" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="U127" s="17" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="128" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B128" s="19">
+        <v>43346.998384863648</v>
+      </c>
+      <c r="C128" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D128" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E128" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="F128" s="17" t="s">
+        <v>363</v>
+      </c>
+      <c r="G128" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="H128" s="17" t="s">
+        <v>365</v>
+      </c>
+      <c r="I128" s="17">
+        <v>252</v>
+      </c>
+      <c r="J128" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K128" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="L128" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M128" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="N128" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="O128" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="P128" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q128" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="R128" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="S128" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="T128" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="U128" s="17" t="s">
         <v>134</v>
       </c>
     </row>
@@ -6328,8 +7312,19 @@
     <hyperlink ref="D110" r:id="rId66"/>
     <hyperlink ref="D111" r:id="rId67"/>
     <hyperlink ref="D112" r:id="rId68"/>
+    <hyperlink ref="D116" r:id="rId69"/>
+    <hyperlink ref="D117" r:id="rId70"/>
+    <hyperlink ref="D118" r:id="rId71"/>
+    <hyperlink ref="D119" r:id="rId72"/>
+    <hyperlink ref="D120" r:id="rId73"/>
+    <hyperlink ref="L116" r:id="rId74"/>
+    <hyperlink ref="D124" r:id="rId75"/>
+    <hyperlink ref="D125" r:id="rId76"/>
+    <hyperlink ref="D126" r:id="rId77"/>
+    <hyperlink ref="D127" r:id="rId78"/>
+    <hyperlink ref="D128" r:id="rId79"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId69"/>
+  <pageSetup orientation="portrait" r:id="rId80"/>
 </worksheet>
 </file>
</xml_diff>